<commit_message>
Link given to all forms in the master form and sheet updated today
Link given to all forms in the master form
</commit_message>
<xml_diff>
--- a/Requirement.xlsx
+++ b/Requirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kavitha\Documents\GitHub\Web-application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5464C4-77A4-4D56-AF31-449ECCBB4F7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F0195D-F104-4811-A655-7AAD0A5AE010}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="398">
   <si>
     <t>Requirement Master</t>
   </si>
@@ -1230,6 +1230,9 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Test_Student_Registration_Form</t>
   </si>
 </sst>
 </file>
@@ -1368,16 +1371,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1659,10 +1662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F9"/>
+  <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,12 +1718,18 @@
         <v>213</v>
       </c>
     </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" location="'Student Registration Form'!A1" display="Student Registration Form" xr:uid="{5D9501A2-2016-4E18-A20C-F6F07BA2A40A}"/>
     <hyperlink ref="B5" location="'Login Form'!A1" tooltip="Login Form" display="Login Form" xr:uid="{AA5A0856-288C-4DDC-9C66-4E773D0D4794}"/>
     <hyperlink ref="B7" location="'Profile Form'!A1" tooltip="Profile Form" display="Profile Form" xr:uid="{84C990FC-C434-42EE-B82B-117765809ABD}"/>
     <hyperlink ref="B9" location="'Quiz Form'!A1" tooltip="Quiz Form" display="Quiz Form" xr:uid="{8F2916D0-FF5D-4AD3-8C29-348C7C123B1B}"/>
+    <hyperlink ref="B11" location="Test_Student_Registration_Form!A1" tooltip="Test_Student_Registration_Form" display="Test_Student_Registration_Form" xr:uid="{33F2BB7C-FBBA-4560-BCF6-9E66525D664F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1745,14 +1754,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1762,21 +1771,21 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -2027,14 +2036,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2044,21 +2053,21 @@
       <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -2294,9 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952013A2-42AF-458C-9948-4D672B870948}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2384,14 +2391,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2655,14 +2662,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2991,14 +2998,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3230,14 +3237,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3539,14 +3546,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3884,14 +3891,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3902,21 +3909,21 @@
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -3930,7 +3937,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>221</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -4169,14 +4176,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4186,21 +4193,21 @@
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -4453,14 +4460,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -4471,21 +4478,21 @@
       <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -4738,14 +4745,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4755,21 +4762,21 @@
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -5022,14 +5029,14 @@
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -5039,21 +5046,21 @@
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">

</xml_diff>

<commit_message>
Date Of Birth sheet is linked
Date Of Birth sheet is linked with Master sheet
</commit_message>
<xml_diff>
--- a/Requirement.xlsx
+++ b/Requirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kavitha\Documents\GitHub\Web-application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F0195D-F104-4811-A655-7AAD0A5AE010}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C872C64D-A37E-4E95-9D11-AA5B6B643F3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="399">
   <si>
     <t>Requirement Master</t>
   </si>
@@ -1233,6 +1233,9 @@
   </si>
   <si>
     <t>Test_Student_Registration_Form</t>
+  </si>
+  <si>
+    <t>Design Document - Student Registration Form- D.O.B</t>
   </si>
 </sst>
 </file>
@@ -1664,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3221,7 +3224,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3324,7 +3327,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -3523,6 +3526,7 @@
   <hyperlinks>
     <hyperlink ref="A1" location="Master!A1" display="Master" xr:uid="{4D6E3066-9ECF-4BFA-BE3A-3BE7F4EDF5C2}"/>
     <hyperlink ref="B4" location="SR_SRF_001!A1" display="SR_SRF_001" xr:uid="{19B2B29B-9E3C-4774-B982-EAEBC0C7604C}"/>
+    <hyperlink ref="B7" location="SR_SRF_004!A1" display="SR_SRF_004" xr:uid="{A096DDCE-287C-4D48-98AB-9EE22470B122}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -3533,7 +3537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D682DBB-42BE-4AE8-A13D-AC6FEE308162}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3876,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A85634-CA1D-4BDF-91D9-82BD7E5EE0C4}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3892,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>29</v>
+        <v>398</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -4445,9 +4451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986BA68A-71D8-413D-9030-9F44612C1420}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>